<commit_message>
Updated DA Projekt Protokoll
</commit_message>
<xml_diff>
--- a/DA_Protokoll/DA_Projekt_Protokoll_Pruggmayer.xlsx
+++ b/DA_Protokoll/DA_Projekt_Protokoll_Pruggmayer.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Clemens\Schule\_DA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74F8201A-501E-402F-901F-E5184410D460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="945" windowWidth="16725" windowHeight="10695"/>
+    <workbookView xWindow="2505" yWindow="3435" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Begleitprotokoll" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Begleitprotokoll!$A$1:$H$30</definedName>
   </definedNames>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>Name:</t>
   </si>
@@ -308,11 +307,41 @@
   <si>
     <t>SvVis Library auf Interrupts umgeschrieben</t>
   </si>
+  <si>
+    <t>SvVis test server schreiben, C partition Speicherplatz beschaffen</t>
+  </si>
+  <si>
+    <t>Multithread syncronisation testing</t>
+  </si>
+  <si>
+    <t>SvVis Um Sockets erweitert</t>
+  </si>
+  <si>
+    <t>SvVis um Color Themes erweitert</t>
+  </si>
+  <si>
+    <t>SvVis Color Theme Aufgeräumt</t>
+  </si>
+  <si>
+    <t>Cortex Programm auf Neue Pinbelegung umgeschrieben &amp; PWD-Generierung hinzugefügt</t>
+  </si>
+  <si>
+    <t>SvVis Programm Color Theme Fehlerbehebungen</t>
+  </si>
+  <si>
+    <t>Cortex Programm Positions LEDS Ansteuerung</t>
+  </si>
+  <si>
+    <t>SvVis Dark Theme fertig gestellt</t>
+  </si>
+  <si>
+    <t>Software für Fahrzeug PWM mit Hardwaretimer generieren lassen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="h&quot;:&quot;mm"/>
     <numFmt numFmtId="165" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
@@ -748,24 +777,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -797,6 +808,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="14" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,25 +856,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -836,19 +865,19 @@
     <cellStyle name="Accent 1" xfId="8"/>
     <cellStyle name="Accent 2" xfId="9"/>
     <cellStyle name="Accent 3" xfId="10"/>
-    <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Error" xfId="11"/>
     <cellStyle name="Footnote" xfId="12"/>
-    <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="3" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading" xfId="13"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="14"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="6" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="4" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Status" xfId="15"/>
     <cellStyle name="Text" xfId="16"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="2" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Warning" xfId="17"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -865,9 +894,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1228,7 +1257,7 @@
                   <c:v>5.6666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -1237,25 +1266,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>4.5833333333333339</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -1305,6 +1334,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CA33-40F1-9CB2-25D4DB6CD190}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1315,11 +1349,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="353328688"/>
-        <c:axId val="486418416"/>
+        <c:axId val="442392592"/>
+        <c:axId val="441524368"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="486418416"/>
+        <c:axId val="441524368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,12 +1460,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353328688"/>
+        <c:crossAx val="442392592"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="353328688"/>
+        <c:axId val="442392592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1527,7 +1561,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486418416"/>
+        <c:crossAx val="441524368"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1610,7 +1644,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3EDACF-FA42-46C8-B0EF-EA6922CD6E61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE3EDACF-FA42-46C8-B0EF-EA6922CD6E61}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1930,11 +1964,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HZ203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
@@ -1948,62 +1982,62 @@
     <col min="1025" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:234" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+    <row r="1" spans="1:234" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" spans="1:234" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:234" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="2">
         <f>SUM(E5:E203)</f>
-        <v>27.409999999999997</v>
+        <v>32.989999999999995</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F5:F203)</f>
-        <v>111.4233333333333</v>
+        <v>141.42666666666662</v>
       </c>
       <c r="G2" s="3">
         <f>SUM(G5:G203)</f>
-        <v>138.83333333333334</v>
+        <v>174.41666666666669</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:234" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="45" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="1"/>
@@ -2233,21 +2267,21 @@
       <c r="HY3"/>
       <c r="HZ3"/>
     </row>
-    <row r="4" spans="1:234" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="23"/>
+    <row r="4" spans="1:234" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+    </row>
+    <row r="5" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>43950</v>
       </c>
@@ -2276,7 +2310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>43952</v>
       </c>
@@ -2305,7 +2339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43954</v>
       </c>
@@ -2337,7 +2371,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>43956</v>
       </c>
@@ -2366,7 +2400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>43971</v>
       </c>
@@ -2395,7 +2429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>43972</v>
       </c>
@@ -2424,7 +2458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>43973</v>
       </c>
@@ -2453,7 +2487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>43974</v>
       </c>
@@ -2482,7 +2516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>43975</v>
       </c>
@@ -2511,7 +2545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>43992</v>
       </c>
@@ -2540,7 +2574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>43999</v>
       </c>
@@ -2569,7 +2603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:234" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:234" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>44000</v>
       </c>
@@ -2598,7 +2632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>44001</v>
       </c>
@@ -2627,7 +2661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>44011</v>
       </c>
@@ -2656,7 +2690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>44012</v>
       </c>
@@ -2685,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>44020</v>
       </c>
@@ -2714,7 +2748,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>44031</v>
       </c>
@@ -2743,7 +2777,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>44032</v>
       </c>
@@ -2772,7 +2806,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>44035</v>
       </c>
@@ -2801,7 +2835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>44037</v>
       </c>
@@ -2830,7 +2864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>44038</v>
       </c>
@@ -2859,7 +2893,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>44046</v>
       </c>
@@ -2888,7 +2922,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>44047</v>
       </c>
@@ -2917,7 +2951,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>44057</v>
       </c>
@@ -2946,7 +2980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>44066</v>
       </c>
@@ -2975,7 +3009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>44078</v>
       </c>
@@ -3004,7 +3038,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>44079</v>
       </c>
@@ -3033,7 +3067,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>44085</v>
       </c>
@@ -3062,7 +3096,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>44086</v>
       </c>
@@ -3091,7 +3125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>44091</v>
       </c>
@@ -3120,7 +3154,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>44092</v>
       </c>
@@ -3149,7 +3183,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>44092</v>
       </c>
@@ -3178,7 +3212,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>44099</v>
       </c>
@@ -3207,7 +3241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>44106</v>
       </c>
@@ -3236,7 +3270,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>44110</v>
       </c>
@@ -3265,7 +3299,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>44113</v>
       </c>
@@ -3294,7 +3328,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>44113</v>
       </c>
@@ -3323,7 +3357,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>44114</v>
       </c>
@@ -3352,7 +3386,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>44118</v>
       </c>
@@ -3381,7 +3415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>44120</v>
       </c>
@@ -3410,8 +3444,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="52">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="39">
         <v>44123</v>
       </c>
       <c r="B45" s="9">
@@ -3422,214 +3456,314 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D45" s="11">
-        <v>0.54166666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E45" s="13">
         <v>3</v>
       </c>
       <c r="F45" s="13">
         <f t="shared" si="4"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G45" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H45" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="9" t="e">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="39">
+        <v>44148</v>
+      </c>
+      <c r="B46" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="13"/>
+        <v>46</v>
+      </c>
+      <c r="C46" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D46" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="13">
+        <v>0</v>
+      </c>
       <c r="F46" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G46" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H46" s="14"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="9" t="e">
+        <v>4</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="39">
+        <v>44155</v>
+      </c>
+      <c r="B47" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="13"/>
+        <v>47</v>
+      </c>
+      <c r="C47" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E47" s="13">
+        <v>0</v>
+      </c>
       <c r="F47" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G47" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H47" s="14"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="9" t="e">
+        <v>3</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="39">
+        <v>44159</v>
+      </c>
+      <c r="B48" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="C48" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D48" s="11">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E48" s="13">
+        <v>3</v>
+      </c>
       <c r="F48" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G48" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="14"/>
-    </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="9" t="e">
+        <v>5</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="39">
+        <v>44158</v>
+      </c>
+      <c r="B49" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="C49" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E49" s="13">
+        <v>0</v>
+      </c>
       <c r="F49" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H49" s="14"/>
-    </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="9" t="e">
+        <v>3</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="39">
+        <v>44161</v>
+      </c>
+      <c r="B50" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="C50" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="D50" s="11">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E50" s="13">
+        <v>0</v>
+      </c>
       <c r="F50" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G50" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H50" s="14"/>
-    </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="9" t="e">
+        <v>2</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="39">
+        <v>44162</v>
+      </c>
+      <c r="B51" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="C51" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D51" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E51" s="13">
+        <v>0</v>
+      </c>
       <c r="F51" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G51" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="9" t="e">
+        <v>3</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="39">
+        <v>44166</v>
+      </c>
+      <c r="B52" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="C52" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E52" s="13">
+        <v>0</v>
+      </c>
       <c r="F52" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G52" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H52" s="14"/>
-    </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="9" t="e">
+        <v>4</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="39">
+        <v>44179</v>
+      </c>
+      <c r="B53" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="C53" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E53" s="13">
+        <v>0</v>
+      </c>
       <c r="F53" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G53" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H53" s="14"/>
-    </row>
-    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="9" t="e">
+        <v>2</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="39">
+        <v>44180</v>
+      </c>
+      <c r="B54" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="C54" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D54" s="11">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="E54" s="13">
+        <v>2.58</v>
+      </c>
       <c r="F54" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.3333333333334103E-3</v>
       </c>
       <c r="G54" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="14"/>
-    </row>
-    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="9" t="e">
+        <v>2.5833333333333335</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="39">
+        <v>44191</v>
+      </c>
+      <c r="B55" s="9">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="C55" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="D55" s="11">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E55" s="13">
+        <v>0</v>
+      </c>
       <c r="F55" s="13">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G55" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H55" s="14"/>
-    </row>
-    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="17"/>
       <c r="B56" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3648,7 +3782,7 @@
       </c>
       <c r="H56" s="14"/>
     </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
       <c r="B57" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3667,7 +3801,7 @@
       </c>
       <c r="H57" s="14"/>
     </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="17"/>
       <c r="B58" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3686,7 +3820,7 @@
       </c>
       <c r="H58" s="14"/>
     </row>
-    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="17"/>
       <c r="B59" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3705,7 +3839,7 @@
       </c>
       <c r="H59" s="14"/>
     </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="17"/>
       <c r="B60" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3724,7 +3858,7 @@
       </c>
       <c r="H60" s="14"/>
     </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="17"/>
       <c r="B61" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3743,7 +3877,7 @@
       </c>
       <c r="H61" s="14"/>
     </row>
-    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="17"/>
       <c r="B62" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3762,7 +3896,7 @@
       </c>
       <c r="H62" s="14"/>
     </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="17"/>
       <c r="B63" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3781,7 +3915,7 @@
       </c>
       <c r="H63" s="14"/>
     </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="17"/>
       <c r="B64" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3800,7 +3934,7 @@
       </c>
       <c r="H64" s="14"/>
     </row>
-    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="17"/>
       <c r="B65" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3819,7 +3953,7 @@
       </c>
       <c r="H65" s="14"/>
     </row>
-    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="17"/>
       <c r="B66" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3838,7 +3972,7 @@
       </c>
       <c r="H66" s="14"/>
     </row>
-    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3857,7 +3991,7 @@
       </c>
       <c r="H67" s="14"/>
     </row>
-    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="9" t="e">
         <f t="shared" si="3"/>
@@ -3876,7 +4010,7 @@
       </c>
       <c r="H68" s="14"/>
     </row>
-    <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="9" t="e">
         <f t="shared" ref="B69:B100" si="6">TRUNC((A69-DATE(YEAR(A69+3-MOD(A69-2,7)),1,MOD(A69-2,7)-9))/7)</f>
@@ -3895,7 +4029,7 @@
       </c>
       <c r="H69" s="14"/>
     </row>
-    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="17"/>
       <c r="B70" s="9" t="e">
         <f t="shared" si="6"/>
@@ -3914,7 +4048,7 @@
       </c>
       <c r="H70" s="14"/>
     </row>
-    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="17"/>
       <c r="B71" s="9" t="e">
         <f t="shared" si="6"/>
@@ -3933,7 +4067,7 @@
       </c>
       <c r="H71" s="14"/>
     </row>
-    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="17"/>
       <c r="B72" s="9" t="e">
         <f t="shared" si="6"/>
@@ -3952,7 +4086,7 @@
       </c>
       <c r="H72" s="14"/>
     </row>
-    <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="17"/>
       <c r="B73" s="9" t="e">
         <f t="shared" si="6"/>
@@ -3971,7 +4105,7 @@
       </c>
       <c r="H73" s="14"/>
     </row>
-    <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="17"/>
       <c r="B74" s="9" t="e">
         <f t="shared" si="6"/>
@@ -3990,7 +4124,7 @@
       </c>
       <c r="H74" s="14"/>
     </row>
-    <row r="75" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="17"/>
       <c r="B75" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4009,7 +4143,7 @@
       </c>
       <c r="H75" s="14"/>
     </row>
-    <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="17"/>
       <c r="B76" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4028,7 +4162,7 @@
       </c>
       <c r="H76" s="14"/>
     </row>
-    <row r="77" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="17"/>
       <c r="B77" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4047,7 +4181,7 @@
       </c>
       <c r="H77" s="14"/>
     </row>
-    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="17"/>
       <c r="B78" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4066,7 +4200,7 @@
       </c>
       <c r="H78" s="14"/>
     </row>
-    <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="17"/>
       <c r="B79" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4085,7 +4219,7 @@
       </c>
       <c r="H79" s="14"/>
     </row>
-    <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="17"/>
       <c r="B80" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4104,7 +4238,7 @@
       </c>
       <c r="H80" s="14"/>
     </row>
-    <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="17"/>
       <c r="B81" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4123,7 +4257,7 @@
       </c>
       <c r="H81" s="14"/>
     </row>
-    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="17"/>
       <c r="B82" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4142,7 +4276,7 @@
       </c>
       <c r="H82" s="14"/>
     </row>
-    <row r="83" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="17"/>
       <c r="B83" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4161,7 +4295,7 @@
       </c>
       <c r="H83" s="14"/>
     </row>
-    <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="17"/>
       <c r="B84" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4180,7 +4314,7 @@
       </c>
       <c r="H84" s="14"/>
     </row>
-    <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="17"/>
       <c r="B85" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4199,7 +4333,7 @@
       </c>
       <c r="H85" s="14"/>
     </row>
-    <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="17"/>
       <c r="B86" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4218,7 +4352,7 @@
       </c>
       <c r="H86" s="14"/>
     </row>
-    <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="17"/>
       <c r="B87" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4237,7 +4371,7 @@
       </c>
       <c r="H87" s="14"/>
     </row>
-    <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="17"/>
       <c r="B88" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4256,7 +4390,7 @@
       </c>
       <c r="H88" s="14"/>
     </row>
-    <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="17"/>
       <c r="B89" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4275,7 +4409,7 @@
       </c>
       <c r="H89" s="14"/>
     </row>
-    <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="17"/>
       <c r="B90" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4294,7 +4428,7 @@
       </c>
       <c r="H90" s="14"/>
     </row>
-    <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="17"/>
       <c r="B91" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4313,7 +4447,7 @@
       </c>
       <c r="H91" s="14"/>
     </row>
-    <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="17"/>
       <c r="B92" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4332,7 +4466,7 @@
       </c>
       <c r="H92" s="14"/>
     </row>
-    <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="17"/>
       <c r="B93" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4351,7 +4485,7 @@
       </c>
       <c r="H93" s="14"/>
     </row>
-    <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="17"/>
       <c r="B94" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4370,7 +4504,7 @@
       </c>
       <c r="H94" s="14"/>
     </row>
-    <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="17"/>
       <c r="B95" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4389,7 +4523,7 @@
       </c>
       <c r="H95" s="14"/>
     </row>
-    <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="17"/>
       <c r="B96" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4408,7 +4542,7 @@
       </c>
       <c r="H96" s="14"/>
     </row>
-    <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4427,7 +4561,7 @@
       </c>
       <c r="H97" s="14"/>
     </row>
-    <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="17"/>
       <c r="B98" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4446,7 +4580,7 @@
       </c>
       <c r="H98" s="14"/>
     </row>
-    <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="17"/>
       <c r="B99" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4465,7 +4599,7 @@
       </c>
       <c r="H99" s="14"/>
     </row>
-    <row r="100" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="17"/>
       <c r="B100" s="9" t="e">
         <f t="shared" si="6"/>
@@ -4484,7 +4618,7 @@
       </c>
       <c r="H100" s="14"/>
     </row>
-    <row r="101" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="17"/>
       <c r="B101" s="9" t="e">
         <f t="shared" ref="B101:B132" si="9">TRUNC((A101-DATE(YEAR(A101+3-MOD(A101-2,7)),1,MOD(A101-2,7)-9))/7)</f>
@@ -4503,7 +4637,7 @@
       </c>
       <c r="H101" s="18"/>
     </row>
-    <row r="102" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="17"/>
       <c r="B102" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4522,7 +4656,7 @@
       </c>
       <c r="H102" s="14"/>
     </row>
-    <row r="103" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="17"/>
       <c r="B103" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4541,7 +4675,7 @@
       </c>
       <c r="H103" s="14"/>
     </row>
-    <row r="104" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="17"/>
       <c r="B104" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4560,7 +4694,7 @@
       </c>
       <c r="H104" s="14"/>
     </row>
-    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="17"/>
       <c r="B105" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4579,7 +4713,7 @@
       </c>
       <c r="H105" s="14"/>
     </row>
-    <row r="106" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="17"/>
       <c r="B106" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4598,7 +4732,7 @@
       </c>
       <c r="H106" s="14"/>
     </row>
-    <row r="107" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="17"/>
       <c r="B107" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4617,7 +4751,7 @@
       </c>
       <c r="H107" s="14"/>
     </row>
-    <row r="108" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="17"/>
       <c r="B108" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4636,7 +4770,7 @@
       </c>
       <c r="H108" s="14"/>
     </row>
-    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="17"/>
       <c r="B109" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4655,7 +4789,7 @@
       </c>
       <c r="H109" s="14"/>
     </row>
-    <row r="110" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="17"/>
       <c r="B110" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4674,7 +4808,7 @@
       </c>
       <c r="H110" s="14"/>
     </row>
-    <row r="111" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="17"/>
       <c r="B111" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4693,7 +4827,7 @@
       </c>
       <c r="H111" s="14"/>
     </row>
-    <row r="112" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="17"/>
       <c r="B112" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4712,7 +4846,7 @@
       </c>
       <c r="H112" s="14"/>
     </row>
-    <row r="113" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="17"/>
       <c r="B113" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4731,7 +4865,7 @@
       </c>
       <c r="H113" s="14"/>
     </row>
-    <row r="114" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="17"/>
       <c r="B114" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4750,7 +4884,7 @@
       </c>
       <c r="H114" s="14"/>
     </row>
-    <row r="115" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="17"/>
       <c r="B115" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4769,7 +4903,7 @@
       </c>
       <c r="H115" s="14"/>
     </row>
-    <row r="116" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="17"/>
       <c r="B116" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4788,7 +4922,7 @@
       </c>
       <c r="H116" s="14"/>
     </row>
-    <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="17"/>
       <c r="B117" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4807,7 +4941,7 @@
       </c>
       <c r="H117" s="14"/>
     </row>
-    <row r="118" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="17"/>
       <c r="B118" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4826,7 +4960,7 @@
       </c>
       <c r="H118" s="14"/>
     </row>
-    <row r="119" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="17"/>
       <c r="B119" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4845,7 +4979,7 @@
       </c>
       <c r="H119" s="14"/>
     </row>
-    <row r="120" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="17"/>
       <c r="B120" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4864,7 +4998,7 @@
       </c>
       <c r="H120" s="14"/>
     </row>
-    <row r="121" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="17"/>
       <c r="B121" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4883,7 +5017,7 @@
       </c>
       <c r="H121" s="14"/>
     </row>
-    <row r="122" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="17"/>
       <c r="B122" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4902,7 +5036,7 @@
       </c>
       <c r="H122" s="14"/>
     </row>
-    <row r="123" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="17"/>
       <c r="B123" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4921,7 +5055,7 @@
       </c>
       <c r="H123" s="14"/>
     </row>
-    <row r="124" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="17"/>
       <c r="B124" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4940,7 +5074,7 @@
       </c>
       <c r="H124" s="14"/>
     </row>
-    <row r="125" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="17"/>
       <c r="B125" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4959,7 +5093,7 @@
       </c>
       <c r="H125" s="14"/>
     </row>
-    <row r="126" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="17"/>
       <c r="B126" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4978,7 +5112,7 @@
       </c>
       <c r="H126" s="14"/>
     </row>
-    <row r="127" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="17"/>
       <c r="B127" s="9" t="e">
         <f t="shared" si="9"/>
@@ -4997,7 +5131,7 @@
       </c>
       <c r="H127" s="14"/>
     </row>
-    <row r="128" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="17"/>
       <c r="B128" s="9" t="e">
         <f t="shared" si="9"/>
@@ -5016,7 +5150,7 @@
       </c>
       <c r="H128" s="14"/>
     </row>
-    <row r="129" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="17"/>
       <c r="B129" s="9" t="e">
         <f t="shared" si="9"/>
@@ -5035,7 +5169,7 @@
       </c>
       <c r="H129" s="14"/>
     </row>
-    <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="17"/>
       <c r="B130" s="9" t="e">
         <f t="shared" si="9"/>
@@ -5054,7 +5188,7 @@
       </c>
       <c r="H130" s="14"/>
     </row>
-    <row r="131" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="17"/>
       <c r="B131" s="9" t="e">
         <f t="shared" si="9"/>
@@ -5073,7 +5207,7 @@
       </c>
       <c r="H131" s="14"/>
     </row>
-    <row r="132" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="17"/>
       <c r="B132" s="9" t="e">
         <f t="shared" si="9"/>
@@ -5092,7 +5226,7 @@
       </c>
       <c r="H132" s="14"/>
     </row>
-    <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="17"/>
       <c r="B133" s="9" t="e">
         <f t="shared" ref="B133:B164" si="12">TRUNC((A133-DATE(YEAR(A133+3-MOD(A133-2,7)),1,MOD(A133-2,7)-9))/7)</f>
@@ -5111,7 +5245,7 @@
       </c>
       <c r="H133" s="14"/>
     </row>
-    <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="17"/>
       <c r="B134" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5130,7 +5264,7 @@
       </c>
       <c r="H134" s="14"/>
     </row>
-    <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="17"/>
       <c r="B135" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5149,7 +5283,7 @@
       </c>
       <c r="H135" s="14"/>
     </row>
-    <row r="136" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="17"/>
       <c r="B136" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5168,7 +5302,7 @@
       </c>
       <c r="H136" s="14"/>
     </row>
-    <row r="137" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="17"/>
       <c r="B137" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5187,7 +5321,7 @@
       </c>
       <c r="H137" s="14"/>
     </row>
-    <row r="138" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="17"/>
       <c r="B138" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5206,7 +5340,7 @@
       </c>
       <c r="H138" s="14"/>
     </row>
-    <row r="139" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="17"/>
       <c r="B139" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5225,7 +5359,7 @@
       </c>
       <c r="H139" s="14"/>
     </row>
-    <row r="140" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="17"/>
       <c r="B140" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5244,7 +5378,7 @@
       </c>
       <c r="H140" s="14"/>
     </row>
-    <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="17"/>
       <c r="B141" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5263,7 +5397,7 @@
       </c>
       <c r="H141" s="14"/>
     </row>
-    <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="17"/>
       <c r="B142" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5282,7 +5416,7 @@
       </c>
       <c r="H142" s="14"/>
     </row>
-    <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="17"/>
       <c r="B143" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5301,7 +5435,7 @@
       </c>
       <c r="H143" s="14"/>
     </row>
-    <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="17"/>
       <c r="B144" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5320,7 +5454,7 @@
       </c>
       <c r="H144" s="14"/>
     </row>
-    <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="17"/>
       <c r="B145" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5339,7 +5473,7 @@
       </c>
       <c r="H145" s="14"/>
     </row>
-    <row r="146" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="17"/>
       <c r="B146" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5358,7 +5492,7 @@
       </c>
       <c r="H146" s="14"/>
     </row>
-    <row r="147" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="17"/>
       <c r="B147" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5377,7 +5511,7 @@
       </c>
       <c r="H147" s="14"/>
     </row>
-    <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="17"/>
       <c r="B148" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5396,7 +5530,7 @@
       </c>
       <c r="H148" s="14"/>
     </row>
-    <row r="149" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="17"/>
       <c r="B149" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5415,7 +5549,7 @@
       </c>
       <c r="H149" s="14"/>
     </row>
-    <row r="150" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="17"/>
       <c r="B150" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5434,7 +5568,7 @@
       </c>
       <c r="H150" s="14"/>
     </row>
-    <row r="151" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="17"/>
       <c r="B151" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5453,7 +5587,7 @@
       </c>
       <c r="H151" s="14"/>
     </row>
-    <row r="152" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="17"/>
       <c r="B152" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5472,7 +5606,7 @@
       </c>
       <c r="H152" s="14"/>
     </row>
-    <row r="153" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="17"/>
       <c r="B153" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5491,7 +5625,7 @@
       </c>
       <c r="H153" s="14"/>
     </row>
-    <row r="154" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="17"/>
       <c r="B154" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5510,7 +5644,7 @@
       </c>
       <c r="H154" s="14"/>
     </row>
-    <row r="155" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="17"/>
       <c r="B155" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5529,7 +5663,7 @@
       </c>
       <c r="H155" s="14"/>
     </row>
-    <row r="156" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="17"/>
       <c r="B156" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5548,7 +5682,7 @@
       </c>
       <c r="H156" s="14"/>
     </row>
-    <row r="157" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="17"/>
       <c r="B157" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5567,7 +5701,7 @@
       </c>
       <c r="H157" s="14"/>
     </row>
-    <row r="158" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="17"/>
       <c r="B158" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5586,7 +5720,7 @@
       </c>
       <c r="H158" s="14"/>
     </row>
-    <row r="159" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="17"/>
       <c r="B159" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5605,7 +5739,7 @@
       </c>
       <c r="H159" s="14"/>
     </row>
-    <row r="160" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="17"/>
       <c r="B160" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5624,7 +5758,7 @@
       </c>
       <c r="H160" s="14"/>
     </row>
-    <row r="161" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="17"/>
       <c r="B161" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5643,7 +5777,7 @@
       </c>
       <c r="H161" s="14"/>
     </row>
-    <row r="162" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="17"/>
       <c r="B162" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5662,7 +5796,7 @@
       </c>
       <c r="H162" s="14"/>
     </row>
-    <row r="163" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="17"/>
       <c r="B163" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5681,7 +5815,7 @@
       </c>
       <c r="H163" s="14"/>
     </row>
-    <row r="164" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="17"/>
       <c r="B164" s="9" t="e">
         <f t="shared" si="12"/>
@@ -5700,7 +5834,7 @@
       </c>
       <c r="H164" s="14"/>
     </row>
-    <row r="165" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="17"/>
       <c r="B165" s="9" t="e">
         <f t="shared" ref="B165:B196" si="15">TRUNC((A165-DATE(YEAR(A165+3-MOD(A165-2,7)),1,MOD(A165-2,7)-9))/7)</f>
@@ -5719,7 +5853,7 @@
       </c>
       <c r="H165" s="14"/>
     </row>
-    <row r="166" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="17"/>
       <c r="B166" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5738,7 +5872,7 @@
       </c>
       <c r="H166" s="14"/>
     </row>
-    <row r="167" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="17"/>
       <c r="B167" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5757,7 +5891,7 @@
       </c>
       <c r="H167" s="14"/>
     </row>
-    <row r="168" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="17"/>
       <c r="B168" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5776,7 +5910,7 @@
       </c>
       <c r="H168" s="14"/>
     </row>
-    <row r="169" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="17"/>
       <c r="B169" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5795,7 +5929,7 @@
       </c>
       <c r="H169" s="14"/>
     </row>
-    <row r="170" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="17"/>
       <c r="B170" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5814,7 +5948,7 @@
       </c>
       <c r="H170" s="14"/>
     </row>
-    <row r="171" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="17"/>
       <c r="B171" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5833,7 +5967,7 @@
       </c>
       <c r="H171" s="14"/>
     </row>
-    <row r="172" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="17"/>
       <c r="B172" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5852,7 +5986,7 @@
       </c>
       <c r="H172" s="14"/>
     </row>
-    <row r="173" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="17"/>
       <c r="B173" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5871,7 +6005,7 @@
       </c>
       <c r="H173" s="14"/>
     </row>
-    <row r="174" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="17"/>
       <c r="B174" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5890,7 +6024,7 @@
       </c>
       <c r="H174" s="14"/>
     </row>
-    <row r="175" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="17"/>
       <c r="B175" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5909,7 +6043,7 @@
       </c>
       <c r="H175" s="14"/>
     </row>
-    <row r="176" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="17"/>
       <c r="B176" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5928,7 +6062,7 @@
       </c>
       <c r="H176" s="14"/>
     </row>
-    <row r="177" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="17"/>
       <c r="B177" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5947,7 +6081,7 @@
       </c>
       <c r="H177" s="14"/>
     </row>
-    <row r="178" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="17"/>
       <c r="B178" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5966,7 +6100,7 @@
       </c>
       <c r="H178" s="14"/>
     </row>
-    <row r="179" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="17"/>
       <c r="B179" s="9" t="e">
         <f t="shared" si="15"/>
@@ -5985,7 +6119,7 @@
       </c>
       <c r="H179" s="14"/>
     </row>
-    <row r="180" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="17"/>
       <c r="B180" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6004,7 +6138,7 @@
       </c>
       <c r="H180" s="14"/>
     </row>
-    <row r="181" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="17"/>
       <c r="B181" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6023,7 +6157,7 @@
       </c>
       <c r="H181" s="14"/>
     </row>
-    <row r="182" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="17"/>
       <c r="B182" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6042,7 +6176,7 @@
       </c>
       <c r="H182" s="14"/>
     </row>
-    <row r="183" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="17"/>
       <c r="B183" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6061,7 +6195,7 @@
       </c>
       <c r="H183" s="14"/>
     </row>
-    <row r="184" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="17"/>
       <c r="B184" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6080,7 +6214,7 @@
       </c>
       <c r="H184" s="14"/>
     </row>
-    <row r="185" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="17"/>
       <c r="B185" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6099,7 +6233,7 @@
       </c>
       <c r="H185" s="14"/>
     </row>
-    <row r="186" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="17"/>
       <c r="B186" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6118,7 +6252,7 @@
       </c>
       <c r="H186" s="14"/>
     </row>
-    <row r="187" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="17"/>
       <c r="B187" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6137,7 +6271,7 @@
       </c>
       <c r="H187" s="14"/>
     </row>
-    <row r="188" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="17"/>
       <c r="B188" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6156,7 +6290,7 @@
       </c>
       <c r="H188" s="14"/>
     </row>
-    <row r="189" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="17"/>
       <c r="B189" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6175,7 +6309,7 @@
       </c>
       <c r="H189" s="14"/>
     </row>
-    <row r="190" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="17"/>
       <c r="B190" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6194,7 +6328,7 @@
       </c>
       <c r="H190" s="14"/>
     </row>
-    <row r="191" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="17"/>
       <c r="B191" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6213,7 +6347,7 @@
       </c>
       <c r="H191" s="14"/>
     </row>
-    <row r="192" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="17"/>
       <c r="B192" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6232,7 +6366,7 @@
       </c>
       <c r="H192" s="14"/>
     </row>
-    <row r="193" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="17"/>
       <c r="B193" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6251,7 +6385,7 @@
       </c>
       <c r="H193" s="14"/>
     </row>
-    <row r="194" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="17"/>
       <c r="B194" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6270,7 +6404,7 @@
       </c>
       <c r="H194" s="14"/>
     </row>
-    <row r="195" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="17"/>
       <c r="B195" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6289,7 +6423,7 @@
       </c>
       <c r="H195" s="14"/>
     </row>
-    <row r="196" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="17"/>
       <c r="B196" s="9" t="e">
         <f t="shared" si="15"/>
@@ -6308,17 +6442,17 @@
       </c>
       <c r="H196" s="14"/>
     </row>
-    <row r="197" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="17"/>
       <c r="B197" s="9" t="e">
-        <f t="shared" ref="B197:B228" si="18">TRUNC((A197-DATE(YEAR(A197+3-MOD(A197-2,7)),1,MOD(A197-2,7)-9))/7)</f>
+        <f t="shared" ref="B197:B203" si="18">TRUNC((A197-DATE(YEAR(A197+3-MOD(A197-2,7)),1,MOD(A197-2,7)-9))/7)</f>
         <v>#NUM!</v>
       </c>
       <c r="C197" s="10"/>
       <c r="D197" s="11"/>
       <c r="E197" s="13"/>
       <c r="F197" s="13">
-        <f t="shared" ref="F197:F228" si="19">G197-E197</f>
+        <f t="shared" ref="F197:F203" si="19">G197-E197</f>
         <v>0</v>
       </c>
       <c r="G197" s="12">
@@ -6327,7 +6461,7 @@
       </c>
       <c r="H197" s="14"/>
     </row>
-    <row r="198" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="17"/>
       <c r="B198" s="9" t="e">
         <f t="shared" si="18"/>
@@ -6346,7 +6480,7 @@
       </c>
       <c r="H198" s="14"/>
     </row>
-    <row r="199" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="17"/>
       <c r="B199" s="9" t="e">
         <f t="shared" si="18"/>
@@ -6365,7 +6499,7 @@
       </c>
       <c r="H199" s="14"/>
     </row>
-    <row r="200" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="17"/>
       <c r="B200" s="9" t="e">
         <f t="shared" si="18"/>
@@ -6384,7 +6518,7 @@
       </c>
       <c r="H200" s="14"/>
     </row>
-    <row r="201" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="17"/>
       <c r="B201" s="9" t="e">
         <f t="shared" si="18"/>
@@ -6403,7 +6537,7 @@
       </c>
       <c r="H201" s="14"/>
     </row>
-    <row r="202" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="17"/>
       <c r="B202" s="9" t="e">
         <f t="shared" si="18"/>
@@ -6422,7 +6556,7 @@
       </c>
       <c r="H202" s="14"/>
     </row>
-    <row r="203" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="17"/>
       <c r="B203" s="9" t="e">
         <f t="shared" si="18"/>
@@ -6468,7 +6602,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
@@ -6478,186 +6612,186 @@
     <col min="1025" max="1025" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="26" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:8" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40" t="s">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
     </row>
     <row r="3" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" s="32" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:8" s="26" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="25" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
+      <c r="A7" s="27">
         <v>42900</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="29">
         <v>80</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="29">
         <v>75</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="29">
         <v>70</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36" t="s">
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="37"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="37"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="37"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="37"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="31"/>
     </row>
     <row r="12" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="37"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="31"/>
     </row>
     <row r="13" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="46"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6679,517 +6813,509 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:H63"/>
+  <dimension ref="C8:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C8" s="51" t="s">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="45">
+      <c r="D8" s="52"/>
+      <c r="E8" s="33">
         <f>SUM(D11:D62)</f>
-        <v>138.83333333333331</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="46" t="s">
+        <v>174.41666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C11" s="48">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="36">
         <v>16</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C11,Begleitprotokoll!$G$5:$G$56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C12" s="48">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="36">
         <v>17</v>
       </c>
-      <c r="D12" s="49">
+      <c r="D12" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C12,Begleitprotokoll!$G$5:$G$56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C13" s="48">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="36">
         <v>18</v>
       </c>
-      <c r="D13" s="49">
+      <c r="D13" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C13,Begleitprotokoll!$G$5:$G$56)</f>
         <v>9.5</v>
       </c>
     </row>
-    <row r="14" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="48">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="36">
         <v>19</v>
       </c>
-      <c r="D14" s="49">
+      <c r="D14" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C14,Begleitprotokoll!$G$5:$G$56)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C15" s="48">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="36">
         <v>20</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C15,Begleitprotokoll!$G$5:$G$56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C16" s="48">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="36">
         <v>21</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C16,Begleitprotokoll!$G$5:$G$56)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C17" s="48">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="36">
         <v>22</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C17,Begleitprotokoll!$G$5:$G$56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C18" s="48">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="36">
         <v>23</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C18,Begleitprotokoll!$G$5:$G$56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C19" s="48">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="36">
         <v>24</v>
       </c>
-      <c r="D19" s="49">
+      <c r="D19" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C19,Begleitprotokoll!$G$5:$G$56)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C20" s="48">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="36">
         <v>25</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C20,Begleitprotokoll!$G$5:$G$56)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C21" s="48">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="36">
         <v>26</v>
       </c>
-      <c r="D21" s="49">
+      <c r="D21" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C21,Begleitprotokoll!$G$5:$G$56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C22" s="48">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="36">
         <v>27</v>
       </c>
-      <c r="D22" s="49">
+      <c r="D22" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C22,Begleitprotokoll!$G$5:$G$56)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C23" s="48">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="36">
         <v>28</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$56,Wochenstunden!$C23,Begleitprotokoll!$G$5:$G$56)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C24" s="48">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="36">
         <v>29</v>
       </c>
-      <c r="D24" s="49">
+      <c r="D24" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C24,Begleitprotokoll!$G$5:$G$158)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="3:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="C25" s="48">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="36">
         <v>30</v>
       </c>
-      <c r="D25" s="49">
+      <c r="D25" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C25,Begleitprotokoll!$G$5:$G$158)</f>
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="48">
+      <c r="C26" s="36">
         <v>31</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C26,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="48">
+      <c r="C27" s="36">
         <v>32</v>
       </c>
-      <c r="D27" s="49">
+      <c r="D27" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C27,Begleitprotokoll!$G$5:$G$158)</f>
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="48">
+      <c r="C28" s="36">
         <v>33</v>
       </c>
-      <c r="D28" s="49">
+      <c r="D28" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C28,Begleitprotokoll!$G$5:$G$158)</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="48">
+      <c r="C29" s="36">
         <v>34</v>
       </c>
-      <c r="D29" s="49">
+      <c r="D29" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C29,Begleitprotokoll!$G$5:$G$158)</f>
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" s="48">
+      <c r="C30" s="36">
         <v>35</v>
       </c>
-      <c r="D30" s="49">
+      <c r="D30" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C30,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" s="48">
+      <c r="C31" s="36">
         <v>36</v>
       </c>
-      <c r="D31" s="49">
+      <c r="D31" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C31,Begleitprotokoll!$G$5:$G$158)</f>
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32" s="48">
+      <c r="C32" s="36">
         <v>37</v>
       </c>
-      <c r="D32" s="49">
+      <c r="D32" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C32,Begleitprotokoll!$G$5:$G$158)</f>
         <v>7.333333333333333</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="48">
+      <c r="C33" s="36">
         <v>38</v>
       </c>
-      <c r="D33" s="49">
+      <c r="D33" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C33,Begleitprotokoll!$G$5:$G$158)</f>
         <v>8.75</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="48">
+      <c r="C34" s="36">
         <v>39</v>
       </c>
-      <c r="D34" s="49">
+      <c r="D34" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C34,Begleitprotokoll!$G$5:$G$158)</f>
         <v>5.333333333333333</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="48">
+      <c r="C35" s="36">
         <v>40</v>
       </c>
-      <c r="D35" s="49">
+      <c r="D35" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C35,Begleitprotokoll!$G$5:$G$158)</f>
         <v>5.333333333333333</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="48">
+      <c r="C36" s="36">
         <v>41</v>
       </c>
-      <c r="D36" s="49">
+      <c r="D36" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C36,Begleitprotokoll!$G$5:$G$158)</f>
         <v>10.916666666666666</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="48">
+      <c r="C37" s="36">
         <v>42</v>
       </c>
-      <c r="D37" s="49">
+      <c r="D37" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C37,Begleitprotokoll!$G$5:$G$158)</f>
         <v>5.6666666666666661</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="48">
+      <c r="C38" s="36">
         <v>43</v>
       </c>
-      <c r="D38" s="49">
+      <c r="D38" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C38,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="48">
+      <c r="C39" s="36">
         <v>44</v>
       </c>
-      <c r="D39" s="49">
+      <c r="D39" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C39,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="48">
+      <c r="C40" s="36">
         <v>45</v>
       </c>
-      <c r="D40" s="49">
+      <c r="D40" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C40,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="48">
+      <c r="C41" s="36">
         <v>46</v>
       </c>
-      <c r="D41" s="49">
+      <c r="D41" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C41,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="48">
+      <c r="C42" s="36">
         <v>47</v>
       </c>
-      <c r="D42" s="49">
+      <c r="D42" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C42,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" s="48">
+      <c r="C43" s="36">
         <v>48</v>
       </c>
-      <c r="D43" s="49">
+      <c r="D43" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C43,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" s="48">
+      <c r="C44" s="36">
         <v>49</v>
       </c>
-      <c r="D44" s="49">
+      <c r="D44" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C44,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="48">
+      <c r="C45" s="36">
         <v>50</v>
       </c>
-      <c r="D45" s="49">
+      <c r="D45" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C45,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="48">
+      <c r="C46" s="36">
         <v>51</v>
       </c>
-      <c r="D46" s="49">
+      <c r="D46" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C46,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>4.5833333333333339</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="48">
+      <c r="C47" s="36">
         <v>52</v>
       </c>
-      <c r="D47" s="49">
+      <c r="D47" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C47,Begleitprotokoll!$G$5:$G$158)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="50">
+      <c r="C48" s="38">
         <v>1</v>
       </c>
-      <c r="D48" s="49">
+      <c r="D48" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C48,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="50">
+      <c r="C49" s="38">
         <v>2</v>
       </c>
-      <c r="D49" s="49">
+      <c r="D49" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$158,Wochenstunden!$C49,Begleitprotokoll!$G$5:$G$158)</f>
         <v>0</v>
       </c>
-      <c r="G49" s="49"/>
+      <c r="G49" s="37"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="50">
+      <c r="C50" s="38">
         <v>3</v>
       </c>
-      <c r="D50" s="49">
+      <c r="D50" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C50,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="50">
+      <c r="C51" s="38">
         <v>4</v>
       </c>
-      <c r="D51" s="49">
+      <c r="D51" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C51,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C52" s="50">
+      <c r="C52" s="38">
         <v>5</v>
       </c>
-      <c r="D52" s="49">
+      <c r="D52" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C52,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="50">
+      <c r="C53" s="38">
         <v>6</v>
       </c>
-      <c r="D53" s="49">
+      <c r="D53" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C53,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="50">
+      <c r="C54" s="38">
         <v>7</v>
       </c>
-      <c r="D54" s="49">
+      <c r="D54" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C54,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
-      <c r="G54" s="49"/>
+      <c r="G54" s="37"/>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C55" s="50">
+      <c r="C55" s="38">
         <v>8</v>
       </c>
-      <c r="D55" s="49">
+      <c r="D55" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C55,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
-      <c r="G55" s="49"/>
+      <c r="G55" s="37"/>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C56" s="50">
+      <c r="C56" s="38">
         <v>9</v>
       </c>
-      <c r="D56" s="49">
+      <c r="D56" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C56,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C57" s="50">
+      <c r="C57" s="38">
         <v>10</v>
       </c>
-      <c r="D57" s="49">
+      <c r="D57" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C57,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C58" s="50">
+      <c r="C58" s="38">
         <v>11</v>
       </c>
-      <c r="D58" s="49">
+      <c r="D58" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C58,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
-      <c r="H58" s="49"/>
+      <c r="H58" s="37"/>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C59" s="50">
+      <c r="C59" s="38">
         <v>12</v>
       </c>
-      <c r="D59" s="49">
+      <c r="D59" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$200,Wochenstunden!$C59,Begleitprotokoll!$G$5:$G$200)</f>
         <v>0</v>
       </c>
-      <c r="H59" s="49"/>
+      <c r="H59" s="37"/>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C60" s="50">
+      <c r="C60" s="38">
         <v>13</v>
       </c>
-      <c r="D60" s="49">
+      <c r="D60" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$203,Wochenstunden!$C60,Begleitprotokoll!$G$5:$G$203)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C61" s="50">
+      <c r="C61" s="38">
         <v>14</v>
       </c>
-      <c r="D61" s="49">
+      <c r="D61" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$203,Wochenstunden!$C61,Begleitprotokoll!$G$5:$G$203)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="50">
+      <c r="C62" s="38">
         <v>15</v>
       </c>
-      <c r="D62" s="49">
+      <c r="D62" s="37">
         <f>SUMIF(Begleitprotokoll!$B$5:$B$203,Wochenstunden!$C62,Begleitprotokoll!$G$5:$G$203)</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="49"/>
+      <c r="D63" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>